<commit_message>
adding paper draft check-ins from 2/15
</commit_message>
<xml_diff>
--- a/human_study/data/processed/human_likeness_comment_classifiations.xlsx
+++ b/human_study/data/processed/human_likeness_comment_classifiations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabrice\Documents\GitHub\llm-psych-depth\human_study\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCD7458-A81F-4B70-B91F-FEE5F059F714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4415FD3C-4A34-4B69-8E76-5EF229890794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32145" yWindow="-5040" windowWidth="27675" windowHeight="17880" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31020" yWindow="-3210" windowWidth="28500" windowHeight="17880" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aggregated summary" sheetId="8" r:id="rId1"/>
@@ -1618,13 +1618,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -10488,50 +10488,50 @@
   <sheetData>
     <row r="1" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1"/>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15" t="s">
         <v>300</v>
       </c>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
     </row>
     <row r="2" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="15" t="s">
         <v>295</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14" t="s">
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15" t="s">
         <v>297</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14" t="s">
+      <c r="H2" s="15"/>
+      <c r="I2" s="15" t="s">
         <v>298</v>
       </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14" t="s">
+      <c r="J2" s="15"/>
+      <c r="K2" s="15" t="s">
         <v>299</v>
       </c>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
     </row>
     <row r="3" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -18803,7 +18803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E13C71-092C-4F3C-9923-CBEADECD2D92}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
@@ -18851,12 +18851,12 @@
       <c r="K1" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="14" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>304</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -18887,7 +18887,7 @@
         <v>14</v>
       </c>
       <c r="K2" s="5">
-        <f>SUM(C2:J2)</f>
+        <f t="shared" ref="K2:K18" si="0">SUM(C2:J2)</f>
         <v>65</v>
       </c>
       <c r="M2" t="s">
@@ -18895,7 +18895,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
@@ -18924,7 +18924,7 @@
         <v>13</v>
       </c>
       <c r="K3" s="5">
-        <f>SUM(C3:J3)</f>
+        <f t="shared" si="0"/>
         <v>74</v>
       </c>
       <c r="M3" t="s">
@@ -18932,7 +18932,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="13" t="s">
         <v>2</v>
       </c>
@@ -18961,7 +18961,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="5">
-        <f>SUM(C4:J4)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="M4" t="s">
@@ -18969,7 +18969,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="13" t="s">
         <v>3</v>
       </c>
@@ -18998,12 +18998,12 @@
         <v>0</v>
       </c>
       <c r="K5" s="5">
-        <f>SUM(C5:J5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="13" t="s">
         <v>4</v>
       </c>
@@ -19032,12 +19032,12 @@
         <v>1</v>
       </c>
       <c r="K6" s="5">
-        <f>SUM(C6:J6)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="13" t="s">
         <v>5</v>
       </c>
@@ -19066,12 +19066,12 @@
         <v>0</v>
       </c>
       <c r="K7" s="5">
-        <f>SUM(C7:J7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
@@ -19100,12 +19100,12 @@
         <v>0</v>
       </c>
       <c r="K8" s="5">
-        <f>SUM(C8:J8)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="13" t="s">
         <v>7</v>
       </c>
@@ -19134,12 +19134,12 @@
         <v>0</v>
       </c>
       <c r="K9" s="5">
-        <f>SUM(C9:J9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="13" t="s">
         <v>8</v>
       </c>
@@ -19168,12 +19168,12 @@
         <v>1</v>
       </c>
       <c r="K10" s="5">
-        <f>SUM(C10:J10)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="13" t="s">
         <v>9</v>
       </c>
@@ -19202,12 +19202,12 @@
         <v>1</v>
       </c>
       <c r="K11" s="5">
-        <f>SUM(C11:J11)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="13" t="s">
         <v>10</v>
       </c>
@@ -19236,12 +19236,12 @@
         <v>8</v>
       </c>
       <c r="K12" s="5">
-        <f>SUM(C12:J12)</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="13" t="s">
         <v>11</v>
       </c>
@@ -19270,12 +19270,12 @@
         <v>7</v>
       </c>
       <c r="K13" s="5">
-        <f>SUM(C13:J13)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="13" t="s">
         <v>12</v>
       </c>
@@ -19304,12 +19304,12 @@
         <v>6</v>
       </c>
       <c r="K14" s="5">
-        <f>SUM(C14:J14)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="13" t="s">
         <v>13</v>
       </c>
@@ -19338,12 +19338,12 @@
         <v>6</v>
       </c>
       <c r="K15" s="5">
-        <f>SUM(C15:J15)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="13" t="s">
         <v>247</v>
       </c>
@@ -19372,12 +19372,12 @@
         <v>2</v>
       </c>
       <c r="K16" s="5">
-        <f>SUM(C16:J16)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="13" t="s">
         <v>249</v>
       </c>
@@ -19406,7 +19406,7 @@
         <v>2</v>
       </c>
       <c r="K17" s="5">
-        <f>SUM(C17:J17)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -19440,12 +19440,12 @@
         <v>19</v>
       </c>
       <c r="K18" s="10">
-        <f>SUM(C18:J18)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="16" t="s">
         <v>305</v>
       </c>
       <c r="B19" s="13" t="s">
@@ -19456,665 +19456,665 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="D19" s="11">
-        <f t="shared" ref="D19" si="0">D2/D$18</f>
+        <f t="shared" ref="D19" si="1">D2/D$18</f>
         <v>0.75</v>
       </c>
       <c r="E19" s="11">
-        <f>E2/E$18</f>
+        <f t="shared" ref="E19:F34" si="2">E2/E$18</f>
         <v>1</v>
       </c>
       <c r="F19" s="11">
-        <f>F2/F$18</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="G19" s="11">
-        <f t="shared" ref="G19:K28" si="1">G2/G$18</f>
+        <f t="shared" ref="G19:K28" si="3">G2/G$18</f>
         <v>0.61111111111111116</v>
       </c>
       <c r="H19" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.41176470588235292</v>
       </c>
       <c r="I19" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.55555555555555558</v>
       </c>
       <c r="J19" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.73684210526315785</v>
       </c>
       <c r="K19" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.65</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="11">
-        <f t="shared" ref="C20:D20" si="2">C3/C$18</f>
+        <f t="shared" ref="C20:D20" si="4">C3/C$18</f>
         <v>0.94444444444444442</v>
       </c>
       <c r="D20" s="11">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="E20" s="11">
         <f t="shared" si="2"/>
-        <v>0.75</v>
-      </c>
-      <c r="E20" s="11">
-        <f>E3/E$18</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="F20" s="11">
-        <f>F3/F$18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G20" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="H20" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.6470588235294118</v>
       </c>
       <c r="I20" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.77777777777777779</v>
       </c>
       <c r="J20" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.68421052631578949</v>
       </c>
       <c r="K20" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.74</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="13" t="s">
         <v>2</v>
       </c>
       <c r="C21" s="11">
-        <f t="shared" ref="C21:D21" si="3">C4/C$18</f>
+        <f t="shared" ref="C21:D21" si="5">C4/C$18</f>
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="D21" s="11">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="E21" s="11">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F21" s="11">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G21" s="11">
         <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-      <c r="E21" s="11">
-        <f>E4/E$18</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="F21" s="11">
-        <f>F4/F$18</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G21" s="11">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H21" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I21" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="J21" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K21" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.08</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="13" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="11">
-        <f t="shared" ref="C22:D22" si="4">C5/C$18</f>
+        <f t="shared" ref="C22:D22" si="6">C5/C$18</f>
         <v>0</v>
       </c>
       <c r="D22" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E22" s="11">
-        <f>E5/E$18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F22" s="11">
-        <f>F5/F$18</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="G22" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H22" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I22" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J22" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K22" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.01</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="15"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="13" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="11">
-        <f t="shared" ref="C23:D23" si="5">C6/C$18</f>
+        <f t="shared" ref="C23:D23" si="7">C6/C$18</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="D23" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E23" s="11">
-        <f>E6/E$18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F23" s="11">
-        <f>F6/F$18</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="G23" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H23" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.11764705882352941</v>
       </c>
       <c r="I23" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J23" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.2631578947368418E-2</v>
       </c>
       <c r="K23" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="15"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="11">
-        <f t="shared" ref="C24:D24" si="6">C7/C$18</f>
+        <f t="shared" ref="C24:D24" si="8">C7/C$18</f>
         <v>0</v>
       </c>
       <c r="D24" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E24" s="11">
-        <f>E7/E$18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F24" s="11">
-        <f>F7/F$18</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="G24" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H24" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I24" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J24" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K24" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.01</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="11">
-        <f t="shared" ref="C25:D25" si="7">C8/C$18</f>
+        <f t="shared" ref="C25:D25" si="9">C8/C$18</f>
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="D25" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E25" s="11">
-        <f>E8/E$18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F25" s="11">
-        <f>F8/F$18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G25" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H25" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.11764705882352941</v>
       </c>
       <c r="I25" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J25" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K25" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.03</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="15"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="11">
-        <f t="shared" ref="C26:D26" si="8">C9/C$18</f>
+        <f t="shared" ref="C26:D26" si="10">C9/C$18</f>
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="D26" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="E26" s="11">
-        <f>E9/E$18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F26" s="11">
-        <f>F9/F$18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G26" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H26" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I26" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J26" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K26" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.01</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="11">
-        <f t="shared" ref="C27:D27" si="9">C10/C$18</f>
+        <f t="shared" ref="C27:D27" si="11">C10/C$18</f>
         <v>0</v>
       </c>
       <c r="D27" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="E27" s="11">
-        <f>E10/E$18</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="F27" s="11">
-        <f>F10/F$18</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="G27" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="H27" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I27" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="J27" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.2631578947368418E-2</v>
       </c>
       <c r="K27" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
+      <c r="A28" s="16"/>
       <c r="B28" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="11">
-        <f t="shared" ref="C28:D28" si="10">C11/C$18</f>
+        <f t="shared" ref="C28:D28" si="12">C11/C$18</f>
         <v>0</v>
       </c>
       <c r="D28" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="E28" s="11">
-        <f>E11/E$18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F28" s="11">
-        <f>F11/F$18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G28" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="H28" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I28" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="J28" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.2631578947368418E-2</v>
       </c>
       <c r="K28" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.06</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="15"/>
+      <c r="A29" s="16"/>
       <c r="B29" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C29" s="11">
-        <f t="shared" ref="C29:D29" si="11">C12/C$18</f>
+        <f t="shared" ref="C29:D29" si="13">C12/C$18</f>
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="D29" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="E29" s="11">
-        <f>E12/E$18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F29" s="11">
-        <f>F12/F$18</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="G29" s="11">
-        <f t="shared" ref="G29:K38" si="12">G12/G$18</f>
+        <f t="shared" ref="G29:K34" si="14">G12/G$18</f>
         <v>0.22222222222222221</v>
       </c>
       <c r="H29" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.70588235294117652</v>
       </c>
       <c r="I29" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="J29" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.42105263157894735</v>
       </c>
       <c r="K29" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.38</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="15"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="11">
-        <f t="shared" ref="C30:D30" si="13">C13/C$18</f>
+        <f t="shared" ref="C30:D30" si="15">C13/C$18</f>
         <v>0.1111111111111111</v>
       </c>
       <c r="D30" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.5</v>
       </c>
       <c r="E30" s="11">
-        <f>E13/E$18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F30" s="11">
-        <f>F13/F$18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G30" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="H30" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="I30" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J30" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.36842105263157893</v>
       </c>
       <c r="K30" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.22</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="15"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="13" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="11">
-        <f t="shared" ref="C31:D31" si="14">C14/C$18</f>
+        <f t="shared" ref="C31:D31" si="16">C14/C$18</f>
         <v>0</v>
       </c>
       <c r="D31" s="11">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="E31" s="11">
-        <f>E14/E$18</f>
-        <v>0</v>
-      </c>
-      <c r="F31" s="11">
-        <f>F14/F$18</f>
-        <v>0</v>
-      </c>
-      <c r="G31" s="11">
-        <f t="shared" si="12"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="H31" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.11764705882352941</v>
       </c>
       <c r="I31" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J31" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.31578947368421051</v>
       </c>
       <c r="K31" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.16</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
+      <c r="A32" s="16"/>
       <c r="B32" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="11">
-        <f t="shared" ref="C32:D32" si="15">C15/C$18</f>
+        <f t="shared" ref="C32:D32" si="17">C15/C$18</f>
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="D32" s="11">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0.25</v>
       </c>
       <c r="E32" s="11">
-        <f>E15/E$18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F32" s="11">
-        <f>F15/F$18</f>
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="G32" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="H32" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.52941176470588236</v>
       </c>
       <c r="I32" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="J32" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.31578947368421051</v>
       </c>
       <c r="K32" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.26</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="15"/>
+      <c r="A33" s="16"/>
       <c r="B33" s="13" t="s">
         <v>247</v>
       </c>
       <c r="C33" s="11">
-        <f t="shared" ref="C33:D33" si="16">C16/C$18</f>
+        <f t="shared" ref="C33:D33" si="18">C16/C$18</f>
         <v>0</v>
       </c>
       <c r="D33" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="E33" s="11">
-        <f>E16/E$18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F33" s="11">
-        <f>F16/F$18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G33" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="H33" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.11764705882352941</v>
       </c>
       <c r="I33" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="J33" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.10526315789473684</v>
       </c>
       <c r="K33" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.08</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="15"/>
+      <c r="A34" s="16"/>
       <c r="B34" s="13" t="s">
         <v>249</v>
       </c>
       <c r="C34" s="11">
-        <f t="shared" ref="C34:D34" si="17">C17/C$18</f>
+        <f t="shared" ref="C34:D34" si="19">C17/C$18</f>
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="D34" s="11">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="E34" s="11">
-        <f>E17/E$18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F34" s="11">
-        <f>F17/F$18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G34" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="H34" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="I34" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="J34" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.10526315789473684</v>
       </c>
       <c r="K34" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.12</v>
       </c>
     </row>
@@ -27349,14 +27349,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>271</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="G1" s="14"/>
+      <c r="G1" s="15"/>
       <c r="I1" s="5" t="s">
         <v>273</v>
       </c>
@@ -27802,9 +27802,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Z200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q64" sqref="Q64"/>
+      <selection pane="bottomLeft" activeCell="I205" sqref="I205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28517,7 +28517,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>0</v>
       </c>
@@ -29687,7 +29687,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>0</v>
       </c>
@@ -30389,7 +30389,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>0</v>
       </c>
@@ -32261,7 +32261,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>0</v>
       </c>
@@ -32495,7 +32495,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>0</v>
       </c>
@@ -32729,7 +32729,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>0</v>
       </c>
@@ -36551,7 +36551,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <v>0</v>
       </c>
@@ -37487,7 +37487,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="125" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
         <v>0</v>
       </c>
@@ -37522,7 +37522,7 @@
         <v>0</v>
       </c>
       <c r="L125" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M125" s="2">
         <v>0</v>
@@ -37565,7 +37565,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="126" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
         <v>1</v>
       </c>
@@ -37799,7 +37799,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="129" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
         <v>0</v>
       </c>
@@ -37840,7 +37840,7 @@
         <v>0</v>
       </c>
       <c r="N129" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O129" s="2">
         <v>0</v>
@@ -37877,7 +37877,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="130" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
         <v>1</v>
       </c>
@@ -41309,7 +41309,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="174" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A174" s="2">
         <v>0</v>
       </c>
@@ -41387,7 +41387,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="175" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A175" s="2">
         <v>0</v>
       </c>
@@ -41465,7 +41465,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="176" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A176" s="2">
         <v>0</v>
       </c>
@@ -41500,7 +41500,7 @@
         <v>0</v>
       </c>
       <c r="L176" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M176" s="2">
         <v>0</v>
@@ -42089,7 +42089,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="184" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A184" s="2">
         <v>1</v>
       </c>
@@ -43417,9 +43417,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:Z200" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="4">
+    <filterColumn colId="23">
       <filters>
-        <filter val="1"/>
+        <filter val="Human-High"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>